<commit_message>
Timers SVD for ESila, VE8, VK014
</commit_message>
<xml_diff>
--- a/SVD_Files/Timer.xlsx
+++ b/SVD_Files/Timer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="259">
   <si>
     <t>0x00</t>
   </si>
@@ -826,12 +826,57 @@
   <si>
     <t xml:space="preserve">3 - Rise in CH3_Inp for Ch1 / Inp4 for Ch2 / Inp1 for Ch3 / Inp2 for Ch4 </t>
   </si>
+  <si>
+    <t>BE8</t>
+  </si>
+  <si>
+    <t>ВК014</t>
+  </si>
+  <si>
+    <t>Esila</t>
+  </si>
+  <si>
+    <t>0x4009_4000</t>
+  </si>
+  <si>
+    <t>0x4009_5000</t>
+  </si>
+  <si>
+    <t>0x4009_6000</t>
+  </si>
+  <si>
+    <t>0x4008_A000</t>
+  </si>
+  <si>
+    <t>0x4008_B000</t>
+  </si>
+  <si>
+    <t>0x4008_C000</t>
+  </si>
+  <si>
+    <t>0x4008_D000</t>
+  </si>
+  <si>
+    <t>0x4008_E000</t>
+  </si>
+  <si>
+    <t>0x4008_F000</t>
+  </si>
+  <si>
+    <t>Timer5</t>
+  </si>
+  <si>
+    <t>Timer6</t>
+  </si>
+  <si>
+    <t>Timers аналогичны 1986ВЕ1Т</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +940,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -916,7 +971,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -939,11 +994,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -992,6 +1056,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1281,7 +1348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
+    <sheetView topLeftCell="A108" workbookViewId="0">
       <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
@@ -2943,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3107,7 +3174,114 @@
       </c>
       <c r="J6" s="5"/>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B16:E16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Timer for ESila added with Timer_Test check
</commit_message>
<xml_diff>
--- a/SVD_Files/Timer.xlsx
+++ b/SVD_Files/Timer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="261">
   <si>
     <t>0x00</t>
   </si>
@@ -873,6 +873,9 @@
   </si>
   <si>
     <t>0..31 - for VE8 (опечатка?)</t>
+  </si>
+  <si>
+    <t>0x4009_7000</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1073,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1361,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1453,7 +1456,7 @@
       <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>259</v>
       </c>
     </row>
@@ -3027,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,8 +3256,8 @@
       <c r="D13" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="E13" s="27" t="s">
-        <v>118</v>
+      <c r="E13" s="15" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3286,12 +3289,12 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>